<commit_message>
New visualisations and corrected signficance testing code
</commit_message>
<xml_diff>
--- a/Stats/QueryReformulation_SiginificanceTests.xlsx
+++ b/Stats/QueryReformulation_SiginificanceTests.xlsx
@@ -481,10 +481,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>-16.19673464171471</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.462876061361129e-52</v>
+      </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -503,10 +507,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>-2.119794591424749</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.034269682695044</v>
+      </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -525,10 +533,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>17.96908920204292</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9.137390640061487e-63</v>
+      </c>
       <c r="F4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -547,10 +559,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>-8.080836272454027</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.847745994947768e-15</v>
+      </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -569,10 +585,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="D6" t="n">
+        <v>-15.91533973033386</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5.377182452185044e-51</v>
+      </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -591,10 +611,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>4.250255048127414</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2.335357180777807e-05</v>
+      </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -613,10 +637,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="D8" t="n">
+        <v>-8.688283675598949</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.48544101614294e-17</v>
+      </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -635,10 +663,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="D9" t="n">
+        <v>10.27924703017757</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.254481241650486e-23</v>
+      </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -657,10 +689,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="D10" t="n">
+        <v>-10.41112586172339</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.617740495550662e-24</v>
+      </c>
       <c r="F10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -679,8 +715,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="D11" t="n">
+        <v>-1.193165866798918</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2330879905488209</v>
+      </c>
       <c r="F11" t="b">
         <v>0</v>
       </c>
@@ -701,10 +741,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="D12" t="n">
+        <v>-7.813173464076295</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.408551833295123e-14</v>
+      </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -723,10 +767,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="n">
+        <v>7.985789372128261</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.826324529013668e-15</v>
+      </c>
       <c r="F13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -745,10 +793,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="D14" t="n">
+        <v>-7.015331649993607</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4.227750712248505e-12</v>
+      </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -767,10 +819,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
+      <c r="D15" t="n">
+        <v>6.222794696752393</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7.177293034283988e-10</v>
+      </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -789,10 +845,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="D16" t="n">
+        <v>4.82139917647365</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.64737129545771e-06</v>
+      </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -811,10 +871,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
+      <c r="D17" t="n">
+        <v>-5.304114817442494</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.394449902328642e-07</v>
+      </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -833,10 +897,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
+      <c r="D18" t="n">
+        <v>2.399911883826625</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.01658141463610778</v>
+      </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -855,10 +923,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>-15.6075138344094</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.657006454929549e-49</v>
+      </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -877,10 +949,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>-6.096860556014323</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1.544027197129014e-09</v>
+      </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -899,10 +975,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>6.188443898265586</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8.857322982773228e-10</v>
+      </c>
       <c r="F21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -921,8 +1001,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
+      <c r="D22" t="n">
+        <v>1.707775417512305</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.08798901897227054</v>
+      </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
@@ -943,10 +1027,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+      <c r="D23" t="n">
+        <v>-6.460695343831752</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.626256821921966e-10</v>
+      </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -965,10 +1053,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>-18.23450732100016</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.427992321896036e-64</v>
+      </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -987,10 +1079,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+      <c r="D25" t="n">
+        <v>17.06522952340124</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.723637416388019e-57</v>
+      </c>
       <c r="F25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1009,8 +1105,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>0.2250180750612635</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.8220112774818291</v>
+      </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
@@ -1031,8 +1131,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+      <c r="D27" t="n">
+        <v>0.7499205288227938</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.4534793138961072</v>
+      </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
@@ -1053,10 +1157,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="D28" t="n">
+        <v>-3.842707772227516</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0001293732666300035</v>
+      </c>
       <c r="F28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1075,10 +1183,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="D29" t="n">
+        <v>-4.875693349755621</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.260925704780753e-06</v>
+      </c>
       <c r="F29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1097,10 +1209,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="D30" t="n">
+        <v>-3.955489096256799</v>
+      </c>
+      <c r="E30" t="n">
+        <v>8.177728052050697e-05</v>
+      </c>
       <c r="F30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1119,10 +1235,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="D31" t="n">
+        <v>-2.887695242452138</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.003964545252956113</v>
+      </c>
       <c r="F31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1141,8 +1261,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="D32" t="n">
+        <v>1.443644508430497</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.1491528198551213</v>
+      </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
@@ -1163,10 +1287,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+      <c r="D33" t="n">
+        <v>-2.473666408995761</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.01353894214005848</v>
+      </c>
       <c r="F33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1185,8 +1313,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>0.5234689639567779</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.6007641538344005</v>
+      </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
@@ -1207,8 +1339,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>1.485983213021384</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.1375993779164931</v>
+      </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
@@ -1229,10 +1365,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>-4.881125352027952</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1.227469223926125e-06</v>
+      </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1251,10 +1391,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>3.658192133561733</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.0002672827961662619</v>
+      </c>
       <c r="F37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1273,10 +1417,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>-15.09662782663752</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.130725566103351e-42</v>
+      </c>
       <c r="F38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1295,10 +1443,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>3.472611848460269</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.0005603126297523855</v>
+      </c>
       <c r="F39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1317,10 +1469,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>14.30924274346889</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.75679240596788e-39</v>
+      </c>
       <c r="F40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1339,10 +1495,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>-16.00378019595684</v>
+      </c>
+      <c r="E41" t="n">
+        <v>8.188869421889893e-47</v>
+      </c>
       <c r="F41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1361,10 +1521,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>-14.2623991208988</v>
+      </c>
+      <c r="E42" t="n">
+        <v>6.052878742278432e-39</v>
+      </c>
       <c r="F42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1383,10 +1547,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>5.360010887530811</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1.275083024712709e-07</v>
+      </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1405,10 +1573,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>-11.76548988695961</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.280598601517217e-28</v>
+      </c>
       <c r="F44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1427,10 +1599,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>14.72589617508293</v>
+      </c>
+      <c r="E45" t="n">
+        <v>5.253477665987129e-41</v>
+      </c>
       <c r="F45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1449,10 +1625,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>-10.25780709531607</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1.582906027752563e-22</v>
+      </c>
       <c r="F46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1471,8 +1651,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>-1.044539741226683</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.2967424966338587</v>
+      </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
@@ -1493,10 +1677,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>-11.25915625275951</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.355809897674623e-26</v>
+      </c>
       <c r="F48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -1515,10 +1703,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+      <c r="D49" t="n">
+        <v>11.04657577879319</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1.594059150975131e-25</v>
+      </c>
       <c r="F49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1537,10 +1729,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>-8.324591871507401</v>
+      </c>
+      <c r="E50" t="n">
+        <v>8.214169929566553e-16</v>
+      </c>
       <c r="F50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -1559,10 +1755,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>7.820617544965836</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3.162635272103824e-14</v>
+      </c>
       <c r="F51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -1581,10 +1781,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>7.399994146515413</v>
+      </c>
+      <c r="E52" t="n">
+        <v>5.835554938218246e-13</v>
+      </c>
       <c r="F52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1603,10 +1807,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>-3.798396814934057</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.0001636268659588302</v>
+      </c>
       <c r="F53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1625,10 +1833,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>5.4776166863653</v>
+      </c>
+      <c r="E54" t="n">
+        <v>6.852241429211566e-08</v>
+      </c>
       <c r="F54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1647,10 +1859,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>-10.31655671197658</v>
+      </c>
+      <c r="E55" t="n">
+        <v>9.571537547301107e-23</v>
+      </c>
       <c r="F55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -1669,10 +1885,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>-10.17960972929951</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.083342570692982e-22</v>
+      </c>
       <c r="F56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -1691,10 +1911,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>11.68538987194245</v>
+      </c>
+      <c r="E57" t="n">
+        <v>4.786056754938556e-28</v>
+      </c>
       <c r="F57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1713,10 +1937,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>2.153519241057014</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.03175721795287327</v>
+      </c>
       <c r="F58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1735,10 +1963,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>-5.665643793467352</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.480744956448428e-08</v>
+      </c>
       <c r="F59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1757,10 +1989,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>-15.92733342443636</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.841576468434244e-46</v>
+      </c>
       <c r="F60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -1779,10 +2015,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>16.05834658374216</v>
+      </c>
+      <c r="E61" t="n">
+        <v>4.588535310758409e-47</v>
+      </c>
       <c r="F61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -1801,10 +2041,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>-7.965973737632594</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1.122809363985598e-14</v>
+      </c>
       <c r="F62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -1823,10 +2067,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>-4.013540299565201</v>
+      </c>
+      <c r="E63" t="n">
+        <v>6.90173917255591e-05</v>
+      </c>
       <c r="F63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -1845,10 +2093,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>11.51973285812914</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2.197205074875898e-27</v>
+      </c>
       <c r="F64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1867,10 +2119,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>-4.581655659005011</v>
+      </c>
+      <c r="E65" t="n">
+        <v>5.837846185453879e-06</v>
+      </c>
       <c r="F65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1889,10 +2145,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>-8.903628764660718</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.0111407307989e-17</v>
+      </c>
       <c r="F66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1911,10 +2171,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>3.560945531793536</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.0004049862656907369</v>
+      </c>
       <c r="F67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1933,8 +2197,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>-1.370649369641182</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.1711017366019309</v>
+      </c>
       <c r="F68" t="b">
         <v>0</v>
       </c>
@@ -1955,8 +2223,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>1.350536843881049</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.1774572198821887</v>
+      </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
@@ -1977,10 +2249,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>-5.143670753274511</v>
+      </c>
+      <c r="E70" t="n">
+        <v>3.880777987140347e-07</v>
+      </c>
       <c r="F70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -1999,8 +2275,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>-0.6784440673128418</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.4978053073972417</v>
+      </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
@@ -2021,8 +2301,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+      <c r="D72" t="n">
+        <v>-1.691535825106178</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.09136011768936432</v>
+      </c>
       <c r="F72" t="b">
         <v>0</v>
       </c>
@@ -2043,8 +2327,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+      <c r="D73" t="n">
+        <v>1.953262044815886</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.0513481558434199</v>
+      </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
@@ -2065,8 +2353,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+      <c r="D74" t="n">
+        <v>-1.880707750972641</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.06059496550407422</v>
+      </c>
       <c r="F74" t="b">
         <v>0</v>
       </c>
@@ -2087,8 +2379,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="D75" t="n">
+        <v>1.443465836576006</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.1495180295564632</v>
+      </c>
       <c r="F75" t="b">
         <v>0</v>
       </c>
@@ -2109,8 +2405,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="D76" t="n">
+        <v>-1.052371631718946</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.2931394332382165</v>
+      </c>
       <c r="F76" t="b">
         <v>0</v>
       </c>
@@ -2131,10 +2431,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+      <c r="D77" t="n">
+        <v>-4.022669313807197</v>
+      </c>
+      <c r="E77" t="n">
+        <v>6.647646519820487e-05</v>
+      </c>
       <c r="F77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -2153,8 +2457,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+      <c r="D78" t="n">
+        <v>-1.660014720190828</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.09754099175134952</v>
+      </c>
       <c r="F78" t="b">
         <v>0</v>
       </c>
@@ -2175,10 +2483,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr"/>
+      <c r="D79" t="n">
+        <v>-11.86793377782273</v>
+      </c>
+      <c r="E79" t="n">
+        <v>8.801489329055845e-29</v>
+      </c>
       <c r="F79" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -2197,8 +2509,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr"/>
-      <c r="E80" t="inlineStr"/>
+      <c r="D80" t="n">
+        <v>1.125119109281735</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.261080529955912</v>
+      </c>
       <c r="F80" t="b">
         <v>0</v>
       </c>
@@ -2219,8 +2535,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr"/>
-      <c r="E81" t="inlineStr"/>
+      <c r="D81" t="n">
+        <v>-0.6213246444747701</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.5346703344609551</v>
+      </c>
       <c r="F81" t="b">
         <v>0</v>
       </c>
@@ -2241,8 +2561,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr"/>
-      <c r="E82" t="inlineStr"/>
+      <c r="D82" t="n">
+        <v>0.4310413232828028</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.6666248361726482</v>
+      </c>
       <c r="F82" t="b">
         <v>0</v>
       </c>
@@ -2263,10 +2587,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+      <c r="D83" t="n">
+        <v>-3.720429253879884</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.0002215286722710386</v>
+      </c>
       <c r="F83" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84">
@@ -2285,10 +2613,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr"/>
-      <c r="E84" t="inlineStr"/>
+      <c r="D84" t="n">
+        <v>-10.66997593596014</v>
+      </c>
+      <c r="E84" t="n">
+        <v>4.470346493124957e-24</v>
+      </c>
       <c r="F84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -2307,10 +2639,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr"/>
+      <c r="D85" t="n">
+        <v>9.119479775699869</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1.861194698337426e-18</v>
+      </c>
       <c r="F85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -2329,8 +2665,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr"/>
+      <c r="D86" t="n">
+        <v>0.306914629762491</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.7590366428647255</v>
+      </c>
       <c r="F86" t="b">
         <v>0</v>
       </c>
@@ -2351,8 +2691,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr"/>
-      <c r="E87" t="inlineStr"/>
+      <c r="D87" t="n">
+        <v>1.425083237759707</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.1547595507355993</v>
+      </c>
       <c r="F87" t="b">
         <v>0</v>
       </c>
@@ -2373,10 +2717,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr"/>
+      <c r="D88" t="n">
+        <v>-6.001997248481303</v>
+      </c>
+      <c r="E88" t="n">
+        <v>3.756604758059976e-09</v>
+      </c>
       <c r="F88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -2395,10 +2743,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr"/>
+      <c r="D89" t="n">
+        <v>-8.779059052996413</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2.650781763841455e-17</v>
+      </c>
       <c r="F89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -2417,10 +2769,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
+      <c r="D90" t="n">
+        <v>-4.971711299928679</v>
+      </c>
+      <c r="E90" t="n">
+        <v>9.146292771430195e-07</v>
+      </c>
       <c r="F90" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -2439,10 +2795,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr"/>
-      <c r="E91" t="inlineStr"/>
+      <c r="D91" t="n">
+        <v>-4.781808364567476</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2.291216823930209e-06</v>
+      </c>
       <c r="F91" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -2461,8 +2821,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr"/>
-      <c r="E92" t="inlineStr"/>
+      <c r="D92" t="n">
+        <v>1.414854034321869</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.1577362570683108</v>
+      </c>
       <c r="F92" t="b">
         <v>0</v>
       </c>
@@ -2483,10 +2847,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
+      <c r="D93" t="n">
+        <v>-2.304312117006939</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.02161577031064433</v>
+      </c>
       <c r="F93" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -2505,8 +2873,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr"/>
+      <c r="D94" t="n">
+        <v>-0.2884659190064461</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.7731101402954939</v>
+      </c>
       <c r="F94" t="b">
         <v>0</v>
       </c>
@@ -2527,8 +2899,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr"/>
+      <c r="D95" t="n">
+        <v>1.419235754203514</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.1564558893003336</v>
+      </c>
       <c r="F95" t="b">
         <v>0</v>
       </c>
@@ -2549,10 +2925,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr"/>
-      <c r="E96" t="inlineStr"/>
+      <c r="D96" t="n">
+        <v>-5.542620669829924</v>
+      </c>
+      <c r="E96" t="n">
+        <v>4.83814178214428e-08</v>
+      </c>
       <c r="F96" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
@@ -2571,10 +2951,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr"/>
-      <c r="E97" t="inlineStr"/>
+      <c r="D97" t="n">
+        <v>3.761588412154988</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.0001889104333729842</v>
+      </c>
       <c r="F97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -2593,8 +2977,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr"/>
-      <c r="E98" t="inlineStr"/>
+      <c r="D98" t="n">
+        <v>0.34689410755154</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.7288174098364302</v>
+      </c>
       <c r="F98" t="b">
         <v>0</v>
       </c>
@@ -2615,8 +3003,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr"/>
-      <c r="E99" t="inlineStr"/>
+      <c r="D99" t="n">
+        <v>-0.3468941075515299</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.7288174098364377</v>
+      </c>
       <c r="F99" t="b">
         <v>0</v>
       </c>
@@ -2659,10 +3051,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr"/>
-      <c r="E101" t="inlineStr"/>
+      <c r="D101" t="n">
+        <v>-3.34521060490165</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.0008842579754991349</v>
+      </c>
       <c r="F101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -2681,10 +3077,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr"/>
+      <c r="D102" t="n">
+        <v>-7.91650325312468</v>
+      </c>
+      <c r="E102" t="n">
+        <v>1.599802301200662e-14</v>
+      </c>
       <c r="F102" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -2703,10 +3103,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr"/>
+      <c r="D103" t="n">
+        <v>-2.93075191145712</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.003536776129874125</v>
+      </c>
       <c r="F103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -2725,8 +3129,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr"/>
+      <c r="D104" t="n">
+        <v>0.619899988758321</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.5356071628363259</v>
+      </c>
       <c r="F104" t="b">
         <v>0</v>
       </c>
@@ -2747,8 +3155,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr"/>
+      <c r="D105" t="n">
+        <v>-1.161452347857856</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.2460143698325469</v>
+      </c>
       <c r="F105" t="b">
         <v>0</v>
       </c>
@@ -2769,8 +3181,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr"/>
+      <c r="D106" t="n">
+        <v>1.609151386391814</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.1082169402150285</v>
+      </c>
       <c r="F106" t="b">
         <v>0</v>
       </c>
@@ -2791,8 +3207,12 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr"/>
+      <c r="D107" t="n">
+        <v>0.621569260568324</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.5345095626984862</v>
+      </c>
       <c r="F107" t="b">
         <v>0</v>
       </c>
@@ -2813,10 +3233,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr"/>
+      <c r="D108" t="n">
+        <v>-2.815005775549782</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.005070857969116009</v>
+      </c>
       <c r="F108" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -2835,10 +3259,14 @@
           <t>T-Test</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr"/>
-      <c r="E109" t="inlineStr"/>
+      <c r="D109" t="n">
+        <v>2.669648492818864</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.007841093674715752</v>
+      </c>
       <c r="F109" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>